<commit_message>
Work on output attrs (typo fixes)
</commit_message>
<xml_diff>
--- a/ATL14_output_attrs.xlsx
+++ b/ATL14_output_attrs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/git_repos/surfacechange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{66A3EC1A-9844-7B4C-BC88-6752C0F2C34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FA40C5-476F-7840-B674-1B87F7FEEAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="4240" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="2460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATL14_output_attrs" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1018,16 +1018,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="31" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>

</xml_diff>